<commit_message>
clarity on residence icb in metadata excel file
</commit_message>
<xml_diff>
--- a/reference files/baseline_extract_meta.xlsx
+++ b/reference files/baseline_extract_meta.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://csucloudservices-my.sharepoint.com/personal/alexander_lawless_mlcsu_nhs_uk/Documents/Work/1. Projects/2024_25/mental_health_shiny_app/nhse_mh_inpat_model/reference files/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Andrew.Hood\OneDrive - Midlands and Lancashire CSU\Working Projects\MH inpat modelling\main repo\nhse_mh_inpat_model\reference files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="5" documentId="8_{BDA33D42-3A69-47AC-9CC4-205E8EEDCC88}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B9417384-B9BB-4C54-B005-EC3BC55DEDB2}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8538234-A26A-492B-89A1-59DB0DD3B0D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{01FA3479-5CA2-470F-B017-4BB0F2949246}"/>
+    <workbookView xWindow="28680" yWindow="1665" windowWidth="29040" windowHeight="15225" xr2:uid="{01FA3479-5CA2-470F-B017-4BB0F2949246}"/>
   </bookViews>
   <sheets>
     <sheet name="baseline_extract_meta" sheetId="1" r:id="rId1"/>
@@ -40,9 +40,6 @@
     <t>NHS code of the ICB in which patient resides at time of admission; based on LSOA.</t>
   </si>
   <si>
-    <t>Raw extract constrained to any midlands resident OR admission to midlands based provider</t>
-  </si>
-  <si>
     <t>residence_icb_name</t>
   </si>
   <si>
@@ -167,6 +164,9 @@
   </si>
   <si>
     <t>Derived from MHS504 and MHS518 tables (MHSDS)</t>
+  </si>
+  <si>
+    <t>Raw extract constrained to any midlands resident OR admission to midlands based provider. Last known LSOA used when missing from record.</t>
   </si>
 </sst>
 </file>
@@ -1030,18 +1030,18 @@
   <dimension ref="A1:D16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="26.77734375" customWidth="1"/>
-    <col min="2" max="2" width="75.88671875" customWidth="1"/>
-    <col min="3" max="3" width="52.109375" customWidth="1"/>
-    <col min="4" max="4" width="26.77734375" customWidth="1"/>
+    <col min="1" max="1" width="26.81640625" customWidth="1"/>
+    <col min="2" max="2" width="75.90625" customWidth="1"/>
+    <col min="3" max="3" width="52.08984375" customWidth="1"/>
+    <col min="4" max="4" width="26.81640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1055,7 +1055,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -1063,164 +1063,164 @@
         <v>5</v>
       </c>
       <c r="D2" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
+      <c r="B3" t="s">
         <v>7</v>
       </c>
-      <c r="B3" t="s">
+      <c r="D3" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
         <v>8</v>
       </c>
-      <c r="D3" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
+      <c r="B4" t="s">
         <v>9</v>
       </c>
-      <c r="B4" t="s">
+      <c r="C4" t="s">
         <v>10</v>
       </c>
-      <c r="C4" t="s">
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
+      <c r="B5" t="s">
         <v>12</v>
       </c>
-      <c r="B5" t="s">
+      <c r="C5" t="s">
         <v>13</v>
       </c>
-      <c r="C5" t="s">
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
+      <c r="B6" t="s">
         <v>15</v>
       </c>
-      <c r="B6" t="s">
+      <c r="C6" t="s">
         <v>16</v>
       </c>
-      <c r="C6" t="s">
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
+      <c r="B7" t="s">
         <v>18</v>
       </c>
-      <c r="B7" t="s">
+      <c r="C7" t="s">
         <v>19</v>
       </c>
-      <c r="C7" t="s">
+      <c r="D7" t="s">
         <v>20</v>
       </c>
-      <c r="D7" t="s">
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
+      <c r="B8" t="s">
         <v>22</v>
       </c>
-      <c r="B8" t="s">
+      <c r="C8" t="s">
         <v>23</v>
       </c>
-      <c r="C8" t="s">
+      <c r="D8" t="s">
         <v>24</v>
       </c>
-      <c r="D8" t="s">
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
+      <c r="B9" t="s">
         <v>26</v>
       </c>
-      <c r="B9" t="s">
+      <c r="C9" t="s">
         <v>27</v>
       </c>
-      <c r="C9" t="s">
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
+      <c r="B10" t="s">
         <v>29</v>
       </c>
-      <c r="B10" t="s">
+      <c r="C10" t="s">
         <v>30</v>
       </c>
-      <c r="C10" t="s">
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A11" t="s">
+      <c r="B11" t="s">
         <v>32</v>
       </c>
-      <c r="B11" t="s">
+      <c r="C11" t="s">
         <v>33</v>
       </c>
-      <c r="C11" t="s">
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A12" t="s">
+      <c r="B12" t="s">
         <v>35</v>
       </c>
-      <c r="B12" t="s">
+      <c r="C12" t="s">
         <v>36</v>
       </c>
-      <c r="C12" t="s">
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A13" t="s">
+      <c r="B13" t="s">
         <v>38</v>
       </c>
-      <c r="B13" t="s">
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A14" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A14" t="s">
+      <c r="B14" t="s">
         <v>40</v>
       </c>
-      <c r="B14" t="s">
+      <c r="D14" t="s">
         <v>41</v>
       </c>
-      <c r="D14" t="s">
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A15" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A15" t="s">
+      <c r="B15" t="s">
         <v>43</v>
       </c>
-      <c r="B15" t="s">
+      <c r="D15" t="s">
         <v>44</v>
       </c>
-      <c r="D15" t="s">
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A16" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A16" t="s">
+      <c r="B16" t="s">
         <v>46</v>
       </c>
-      <c r="B16" t="s">
+      <c r="D16" t="s">
         <v>47</v>
-      </c>
-      <c r="D16" t="s">
-        <v>48</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added note on residence missing data to meta file.
</commit_message>
<xml_diff>
--- a/reference files/baseline_extract_meta.xlsx
+++ b/reference files/baseline_extract_meta.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Andrew.Hood\OneDrive - Midlands and Lancashire CSU\Working Projects\MH inpat modelling\main repo\nhse_mh_inpat_model\reference files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8538234-A26A-492B-89A1-59DB0DD3B0D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9ED731DF-BF7E-461D-ACEC-68BFD76A1DE0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="1665" windowWidth="29040" windowHeight="15225" xr2:uid="{01FA3479-5CA2-470F-B017-4BB0F2949246}"/>
+    <workbookView xWindow="-80" yWindow="-80" windowWidth="19360" windowHeight="10940" xr2:uid="{01FA3479-5CA2-470F-B017-4BB0F2949246}"/>
   </bookViews>
   <sheets>
     <sheet name="baseline_extract_meta" sheetId="1" r:id="rId1"/>
@@ -1029,7 +1029,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D586B6A4-BFFC-439D-84AB-BFCC871E2CAE}">
   <dimension ref="A1:D16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
       <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>

</xml_diff>